<commit_message>
Branch for adding Batterywise analysis!
</commit_message>
<xml_diff>
--- a/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V2/D11_03_2024/B4_BT02_09.56_10.40/analysis_B4_BT02_09.56_10.40.xlsx
+++ b/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V2/D11_03_2024/B4_BT02_09.56_10.40/analysis_B4_BT02_09.56_10.40.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>0.0308222337962963</v>
+        <v>0.0309358912037037</v>
       </c>
     </row>
     <row r="2">
@@ -441,7 +441,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>29.75020694444444</v>
+        <v>29.75749527777777</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1500.779628262778</v>
+        <v>1501.156768779445</v>
       </c>
     </row>
     <row r="4">
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.035</v>
+        <v>9.025</v>
       </c>
     </row>
     <row r="6">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>22</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
@@ -491,33 +491,33 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>98</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Total distance covered (in kilometers)</t>
+          <t>Total distance covered (km)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30.62569010526831</v>
+        <v>30.62844142383255</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WH/KM</t>
+          <t>Total energy consumption(WH/KM)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49.00394482880926</v>
+        <v>49.01185626805572</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Total SOC consumed</t>
+          <t>Total SOC consumed(%)</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -533,9 +533,9 @@
       <c r="B11" t="inlineStr">
         <is>
           <t>Custom mode
-85.04%
+84.72%
 Eco mode
-13.92%
+14.25%
 Sports mode
 0.04%</t>
         </is>
@@ -544,7 +544,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Peak Power</t>
+          <t>Peak Power(kW)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -554,17 +554,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Average Power</t>
+          <t>Average Power(kW)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-2035.722178502638</v>
+        <v>-2028.590228080331</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Total Energy Regenerated</t>
+          <t>Total Energy Regenerated(kWh)</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -574,37 +574,37 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Regenerative Effectiveness</t>
+          <t>Regenerative Effectiveness(%)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.000854977994777095</v>
+        <v>0.0008547631976997756</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Lowest Cell Voltage</t>
+          <t>Highest Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3.017</v>
+        <v>3.329</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Highest Cell Voltage</t>
+          <t>Lowest Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.329</v>
+        <v>3.017</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Difference in Cell Voltage</t>
+          <t>Difference in Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -614,7 +614,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Minimum Temperature</t>
+          <t>Minimum Temperature(C)</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -624,7 +624,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Maximum Temperature</t>
+          <t>Maximum Temperature(C)</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -634,17 +634,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Difference in Temperature</t>
+          <t>Difference in Temperature(C)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v/>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Maximum Fet Temperature</t>
+          <t>Maximum Fet Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -654,7 +654,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Maximum Afe Temperature</t>
+          <t>Maximum Afe Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -664,7 +664,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Maximum PCB Temperature</t>
+          <t>Maximum PCB Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -674,7 +674,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Maximum MCU Temperature</t>
+          <t>Maximum MCU Temperature(C)</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -684,7 +684,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Maximum Motor Temperature</t>
+          <t>Maximum Motor Temperature(C)</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -694,7 +694,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Abnormal Motor Temperature Detected</t>
+          <t>Abnormal Motor Temperature Detected(C)</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -704,7 +704,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>lowest cell temp</t>
+          <t>highest cell temp(C)</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -714,7 +714,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>highest cell temp</t>
+          <t>lowest cell temp(C)</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -724,7 +724,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Difference between Highest and Lowest Cell Temperature at 100% SOC</t>
+          <t>Difference between Highest and Lowest Cell Temperature at 100% SOC(C)</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -734,121 +734,131 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Maximum BMS Temperature in C</t>
+          <t>Battery Voltage(V)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Battery Voltage</t>
+          <t>Total energy charged(kWh)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5.3</v>
+        <v>1.577147249722222</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Total energy charged in kWh</t>
+          <t>Electricity consumption units(kW)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1576760968055556</v>
+        <v>1.63958255335394e-07</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Electricity consumption units in kW</t>
+          <t>Idling time percentage</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1.644720832869733e-08</v>
+        <v>7.848300255452938</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Idling time percentage</t>
+          <t>Time spent in 0-10 km/h</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>6.458357991083758</v>
+        <v>10.55610139516604</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Time spent in 0-10 km/h</t>
+          <t>Time spent in 10-20 km/h</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>16.95269657158638</v>
+        <v>5.380231872666536</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Time spent in 10-20 km/h</t>
+          <t>Time spent in 20-30 km/h</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>5.369471732354913</v>
+        <v>8.630379249361368</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Time spent in 20-30 km/h</t>
+          <t>Time spent in 30-40 km/h</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>8.675582909220026</v>
+        <v>13.29534289644331</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Time spent in 30-40 km/h</t>
+          <t>Time spent in 40-50 km/h</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>13.35858286976762</v>
+        <v>12.1988602868933</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Time spent in 40-50 km/h</t>
+          <t>Time spent in 50-60 km/h</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>12.2775870911745</v>
+        <v>12.58793476124976</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Time spent in 50-60 km/h</t>
+          <t>Time spent in 60-70 km/h</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>12.65633013768888</v>
+        <v>19.68952642955394</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Time spent in 60-70 km/h</t>
+          <t>Time spent in 70-80 km/h</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>19.78143370024066</v>
+        <v>9.660051090587542</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Time spent in 80-90 km/h</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'Date and Time' and 'Cycle_count' parameters
</commit_message>
<xml_diff>
--- a/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V2/D11_03_2024/B4_BT02_09.56_10.40/analysis_B4_BT02_09.56_10.40.xlsx
+++ b/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V2/D11_03_2024/B4_BT02_09.56_10.40/analysis_B4_BT02_09.56_10.40.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,67 +427,69 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Total time taken for the ride</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>0.0308222337962963</v>
+          <t>Date and Time</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2024-03-11 09:55:45.892000 to 2024-03-11 10:40:22.873000</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Actual Ampere-hours (Ah)</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>29.75020694444444</v>
+          <t>Total time taken for the ride</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>0.0308222337962963</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Actual Watt-hours (Wh)</t>
+          <t>Actual Ampere-hours (Ah)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1500.779628262778</v>
+        <v>29.75020694444444</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Starting SoC (Ah)</t>
+          <t>Actual Watt-hours (Wh)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38.875</v>
+        <v>1500.779628262778</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ending SoC (Ah)</t>
+          <t>Starting SoC (Ah)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.035</v>
+        <v>38.875</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Starting SoC (%)</t>
+          <t>Ending SoC (Ah)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>22</v>
+        <v>9.035</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ending SoC (%)</t>
+          <t>Starting SoC (%)</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -497,40 +499,50 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Total distance covered (in kilometers)</t>
+          <t>Ending SoC (%)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30.62569010526831</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>WH/KM</t>
+          <t>Total distance covered (km)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49.00394482880926</v>
+        <v>30.62569010526831</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Total SOC consumed</t>
+          <t>Total energy consumption(WH/KM)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>76</v>
+        <v>49.00394482880926</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Total SOC consumed(%)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>Mode</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Custom mode
 85.04%
@@ -541,60 +553,50 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Peak Power</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>5427.163392</v>
-      </c>
-    </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Average Power</t>
+          <t>Peak Power(kW)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-2035.722178502638</v>
+        <v>5427.163392</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Total Energy Regenerated</t>
+          <t>Average Power(kW)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01283144527777778</v>
+        <v>-2035.722178502638</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Regenerative Effectiveness</t>
+          <t>Total Energy Regenerated(kWh)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.000854977994777095</v>
+        <v>0.01283144527777778</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Lowest Cell Voltage</t>
+          <t>Regenerative Effectiveness(%)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3.017</v>
+        <v>0.000854977994777095</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Highest Cell Voltage</t>
+          <t>Highest Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -604,251 +606,281 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Difference in Cell Voltage</t>
+          <t>Lowest Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.3120000000000003</v>
+        <v>3.017</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Minimum Temperature</t>
+          <t>Difference in Cell Voltage(V)</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>26</v>
+        <v>0.3120000000000003</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Maximum Temperature</t>
+          <t>Minimum Temperature(C)</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Difference in Temperature</t>
+          <t>Maximum Temperature(C)</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v/>
+        <v>40</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Maximum Fet Temperature</t>
+          <t>Difference in Temperature(C)</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>62</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Maximum Afe Temperature</t>
+          <t>Maximum Fet Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Maximum PCB Temperature</t>
+          <t>Maximum Afe Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Maximum MCU Temperature</t>
+          <t>Maximum PCB Temperature-BMS(C)</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Maximum Motor Temperature</t>
+          <t>Maximum MCU Temperature(C)</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>102</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Abnormal Motor Temperature Detected</t>
+          <t>Maximum Motor Temperature(C)</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>lowest cell temp</t>
+          <t>Abnormal Motor Temperature Detected(C)</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>highest cell temp</t>
+          <t>highest cell temp(C)</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Difference between Highest and Lowest Cell Temperature at 100% SOC</t>
+          <t>lowest cell temp(C)</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Maximum BMS Temperature in C</t>
+          <t>Difference between Highest and Lowest Cell Temperature at 100% SOC(C)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Battery Voltage</t>
+          <t>Battery Voltage(V)</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5.3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Total energy charged in kWh</t>
+          <t>Total energy charged(kWh)</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1576760968055556</v>
+        <v>1.576760968055555</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Electricity consumption units in kW</t>
+          <t>Electricity consumption units(kW)</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1.644720832869733e-08</v>
+        <v>1.644720832869733e-07</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Idling time percentage</t>
+          <t>Cycle Count of battery</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>6.458357991083758</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Time spent in 0-10 km/h</t>
+          <t>Idling time percentage</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>16.95269657158638</v>
+        <v>7.641930011441196</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Time spent in 10-20 km/h</t>
+          <t>Time spent in 0-10 km/h</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>5.369471732354913</v>
+        <v>10.49433858050262</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Time spent in 20-30 km/h</t>
+          <t>Time spent in 10-20 km/h</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>8.675582909220026</v>
+        <v>5.353690772083481</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Time spent in 30-40 km/h</t>
+          <t>Time spent in 20-30 km/h</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>13.35858286976762</v>
+        <v>8.663747189016451</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Time spent in 40-50 km/h</t>
+          <t>Time spent in 30-40 km/h</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>12.2775870911745</v>
+        <v>13.34674714956405</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Time spent in 50-60 km/h</t>
+          <t>Time spent in 40-50 km/h</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>12.65633013768888</v>
+        <v>12.24602517063163</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>Time spent in 50-60 km/h</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>12.63660393734959</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>Time spent in 60-70 km/h</t>
         </is>
       </c>
-      <c r="B42" t="n">
-        <v>19.78143370024066</v>
+      <c r="B43" t="n">
+        <v>19.76565273996923</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Time spent in 70-80 km/h</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>9.69740008679528</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Time spent in 80-90 km/h</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>